<commit_message>
update tools and add translation examples
update convert_library.py
translate iso27001-2022
translate risk-matrix 3x3 multiplicative
</commit_message>
<xml_diff>
--- a/tools/matrix/3x3-mult/risk-matrix-3x3-mult.xlsx
+++ b/tools/matrix/3x3-mult/risk-matrix-3x3-mult.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/matrix/3x3-mult/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD08C8A0-C989-9A41-8254-8D82EF52CD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88FE0B4-1DE7-674D-A846-4A1D033ACF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20480" activeTab="1" xr2:uid="{737B4EAE-987D-4047-A963-C4AA7BEFCFC2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20480" xr2:uid="{737B4EAE-987D-4047-A963-C4AA7BEFCFC2}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="85">
   <si>
     <t>library_urn</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Remédiation sous 2 mois</t>
   </si>
   <si>
-    <t>remédiation sour 6 mois</t>
-  </si>
-  <si>
     <t>tolérable</t>
   </si>
   <si>
@@ -205,6 +202,96 @@
   </si>
   <si>
     <t>color</t>
+  </si>
+  <si>
+    <t>name[en]</t>
+  </si>
+  <si>
+    <t>description[en]</t>
+  </si>
+  <si>
+    <t>[3] very likely</t>
+  </si>
+  <si>
+    <t>[2] rather likely</t>
+  </si>
+  <si>
+    <t>[1] unlikely</t>
+  </si>
+  <si>
+    <t>[1] minor</t>
+  </si>
+  <si>
+    <t>[2] moderate</t>
+  </si>
+  <si>
+    <t>[3] major</t>
+  </si>
+  <si>
+    <t>[1] low</t>
+  </si>
+  <si>
+    <t>[2] medium</t>
+  </si>
+  <si>
+    <t>[3] medium</t>
+  </si>
+  <si>
+    <t>[4] medium</t>
+  </si>
+  <si>
+    <t>[6] high</t>
+  </si>
+  <si>
+    <t>[9] critical</t>
+  </si>
+  <si>
+    <t>Remediation within 2 months</t>
+  </si>
+  <si>
+    <t>remediation within 6 months</t>
+  </si>
+  <si>
+    <t>remédiation sous 6 mois</t>
+  </si>
+  <si>
+    <t>tolerable</t>
+  </si>
+  <si>
+    <t>negligible</t>
+  </si>
+  <si>
+    <t>major impact</t>
+  </si>
+  <si>
+    <t>moderate impact</t>
+  </si>
+  <si>
+    <t>minor impact</t>
+  </si>
+  <si>
+    <t>library_name[en]</t>
+  </si>
+  <si>
+    <t>library_description[en]</t>
+  </si>
+  <si>
+    <t>simple 3x3 multiplicative matrix</t>
+  </si>
+  <si>
+    <t>3x3 multiplicative matrix</t>
+  </si>
+  <si>
+    <t>library_copyright[en]</t>
+  </si>
+  <si>
+    <t>public domain</t>
+  </si>
+  <si>
+    <t>risk_matrix_name[en]</t>
+  </si>
+  <si>
+    <t>risk_matrix_description[en]</t>
   </si>
 </sst>
 </file>
@@ -661,15 +748,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF47FB7-BAFE-4E46-A187-08E7F45C581C}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView zoomScale="177" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="111.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -679,7 +766,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -687,7 +774,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -703,7 +790,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -748,7 +835,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
@@ -756,15 +843,15 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
@@ -772,7 +859,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>15</v>
@@ -783,10 +870,50 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -796,10 +923,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C78439-E0E8-6B46-8D3C-6DE0FA8D6D39}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView zoomScale="178" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -810,17 +937,19 @@
     <col min="5" max="5" width="24.1640625" customWidth="1"/>
     <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="10.83203125" style="2"/>
+    <col min="10" max="10" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>17</v>
@@ -840,8 +969,14 @@
       <c r="I1" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -853,7 +988,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
         <v>29</v>
@@ -867,8 +1002,14 @@
       <c r="I2" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -880,7 +1021,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
         <v>28</v>
@@ -894,8 +1035,14 @@
       <c r="I3" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -907,7 +1054,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>
@@ -921,8 +1068,14 @@
       <c r="I4" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -934,13 +1087,19 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -952,13 +1111,19 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -970,13 +1135,19 @@
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -988,13 +1159,19 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="J8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1006,13 +1183,19 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="J9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1024,13 +1207,19 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="J10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1042,13 +1231,19 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="J11" t="s">
+        <v>66</v>
+      </c>
+      <c r="K11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1060,13 +1255,19 @@
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="J12" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1078,10 +1279,16 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F13" t="s">
         <v>30</v>
+      </c>
+      <c r="J13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K13" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>